<commit_message>
adding easier to work with wire frame and updating example rtm with test plan documentation
</commit_message>
<xml_diff>
--- a/Foundation Project/Example RTM.xlsx
+++ b/Foundation Project/Example RTM.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricSuminski\Desktop\240930-JWA\Foundation Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8B9A54-CCBD-4F91-A15E-EC393243AAA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E307E21B-E9AC-4075-A530-9DB3A8C9F8C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D553A7D2-898D-425D-9100-869F82215B38}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{D553A7D2-898D-425D-9100-869F82215B38}"/>
   </bookViews>
   <sheets>
     <sheet name="RTM" sheetId="1" r:id="rId1"/>
+    <sheet name="Strategy" sheetId="2" r:id="rId2"/>
+    <sheet name="Schedule" sheetId="3" r:id="rId3"/>
+    <sheet name="SRS" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>Users should be able to open a new User account with the Planetarium</t>
   </si>
@@ -72,13 +75,91 @@
   </si>
   <si>
     <t>and the user should stay on the registration page</t>
+  </si>
+  <si>
+    <t>ID: 1</t>
+  </si>
+  <si>
+    <t>Boundary Analysis testing for username/password length</t>
+  </si>
+  <si>
+    <t>Equivalence Partition testing for the uniqueness of usernames</t>
+  </si>
+  <si>
+    <t>Exploratory Testing to see if passwords are in plain text in any places we have access to in the provided software</t>
+  </si>
+  <si>
+    <t>Error Guess Testing to see if the passwords are in plain text in the interface for the application a regular user would have access to</t>
+  </si>
+  <si>
+    <t>Error Guess Testing to perform Acceptance Testing for the Use Case</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>1. Requirement Analysis</t>
+  </si>
+  <si>
+    <t>2. Test Planning</t>
+  </si>
+  <si>
+    <t>3. Test Case Development</t>
+  </si>
+  <si>
+    <t>4. Test Environment Setup</t>
+  </si>
+  <si>
+    <t>5. Test Execution</t>
+  </si>
+  <si>
+    <t>6. Test Cycle Closure</t>
+  </si>
+  <si>
+    <t>October 31st</t>
+  </si>
+  <si>
+    <t>October 17th</t>
+  </si>
+  <si>
+    <t>October 21st</t>
+  </si>
+  <si>
+    <t>October 24th</t>
+  </si>
+  <si>
+    <t>October 25th</t>
+  </si>
+  <si>
+    <t>October 30th</t>
+  </si>
+  <si>
+    <t>Completion Target</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>target met</t>
+  </si>
+  <si>
+    <t>target missed</t>
+  </si>
+  <si>
+    <t>target in progress</t>
+  </si>
+  <si>
+    <t>Actual Completion</t>
+  </si>
+  <si>
+    <t>System Requirement Specifications in Foundations Project Document</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,8 +190,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="0.39997558519241921"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,6 +245,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -151,10 +273,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -169,8 +292,46 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -503,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA3B490-9839-44EA-A87B-924B8721CBB2}">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,77 +676,247 @@
     <col min="2" max="2" width="43.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="7" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="10" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="12" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+    <row r="15" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72D5F5EC-3BC4-4B13-BFC6-6AE082A36DC7}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104746C3-76B6-41CE-80DD-9119CA59496B}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A82C953D-5C40-4B49-8BA7-26B2DA71070C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{9F5F385F-336C-40EA-B186-2E4AF0E091B9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updaing rtm example with srs section
</commit_message>
<xml_diff>
--- a/Foundation Project/Example RTM.xlsx
+++ b/Foundation Project/Example RTM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricSuminski\Desktop\240930-JWA\Foundation Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E307E21B-E9AC-4075-A530-9DB3A8C9F8C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145812D3-FC12-468A-A7FE-A9950F4D2603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{D553A7D2-898D-425D-9100-869F82215B38}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>Users should be able to open a new User account with the Planetarium</t>
   </si>
@@ -153,6 +153,18 @@
   </si>
   <si>
     <t>System Requirement Specifications in Foundations Project Document</t>
+  </si>
+  <si>
+    <t>Planetarium Wireframe Documentation</t>
+  </si>
+  <si>
+    <t>Requirements Provided By Stakeholder</t>
+  </si>
+  <si>
+    <t>Setup Script for Planetarium Database</t>
+  </si>
+  <si>
+    <t>Planetarium Application to be Tested</t>
   </si>
 </sst>
 </file>
@@ -214,7 +226,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,8 +275,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -272,12 +290,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -326,9 +359,14 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -899,23 +937,48 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A82C953D-5C40-4B49-8BA7-26B2DA71070C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{9F5F385F-336C-40EA-B186-2E4AF0E091B9}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{9F5F385F-336C-40EA-B186-2E4AF0E091B9}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{BD258779-96B8-4C01-9D6A-E59F283AF271}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{018EDFC1-F08F-4077-91CA-C55372B65EEF}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{F5FE86BE-79B7-4477-BEEA-6B48DB7063FD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding example test case organization for registration use case
</commit_message>
<xml_diff>
--- a/Foundation Project/Example RTM.xlsx
+++ b/Foundation Project/Example RTM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricSuminski\Desktop\240930-JWA\Foundation Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145812D3-FC12-468A-A7FE-A9950F4D2603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E50C9C-F6EA-474A-A91C-2F49D23E7078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{D553A7D2-898D-425D-9100-869F82215B38}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D553A7D2-898D-425D-9100-869F82215B38}"/>
   </bookViews>
   <sheets>
     <sheet name="RTM" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Users should be able to open a new User account with the Planetarium</t>
   </si>
@@ -165,6 +165,12 @@
   </si>
   <si>
     <t>Planetarium Application to be Tested</t>
+  </si>
+  <si>
+    <t>ahead of schedule</t>
+  </si>
+  <si>
+    <t>October 16th</t>
   </si>
 </sst>
 </file>
@@ -226,7 +232,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -281,6 +287,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -310,7 +322,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -344,15 +356,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -367,6 +370,24 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -704,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA3B490-9839-44EA-A87B-924B8721CBB2}">
   <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,6 +812,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -799,7 +821,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,7 +869,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,7 +887,7 @@
       <c r="B1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="13" t="s">
         <v>36</v>
       </c>
       <c r="D1" s="10" t="s">
@@ -873,37 +895,43 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="13" t="s">
+      <c r="C2" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="14" t="s">
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="23" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -912,6 +940,9 @@
       </c>
       <c r="B5" s="8" t="s">
         <v>29</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -939,8 +970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A82C953D-5C40-4B49-8BA7-26B2DA71070C}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,27 +980,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="15" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="17" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="18" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="18" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="16" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding example test case creation documentation to project
</commit_message>
<xml_diff>
--- a/Foundation Project/Example RTM.xlsx
+++ b/Foundation Project/Example RTM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricSuminski\Desktop\240930-JWA\Foundation Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E50C9C-F6EA-474A-A91C-2F49D23E7078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184EC5E3-8F9A-440F-8BB1-49F6E45B53D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D553A7D2-898D-425D-9100-869F82215B38}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{D553A7D2-898D-425D-9100-869F82215B38}"/>
   </bookViews>
   <sheets>
     <sheet name="RTM" sheetId="1" r:id="rId1"/>
@@ -725,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA3B490-9839-44EA-A87B-924B8721CBB2}">
   <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72D5F5EC-3BC4-4B13-BFC6-6AE082A36DC7}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>